<commit_message>
added try except to excel write function
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D85BA7-C93B-4DCD-92BF-A3FE9F1B8DDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80D5FB5-BE5D-4606-9876-FDB7648AF2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -715,7 +715,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K4" s="2">
-        <v>0.4414667568362855</v>
+        <v>0.44146675683628572</v>
       </c>
       <c r="L4" s="2">
         <v>-1.8624580532189181</v>
@@ -774,7 +774,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K5" s="2">
-        <v>-0.12078569171608711</v>
+        <v>-0.120785691716087</v>
       </c>
       <c r="L5" s="2">
         <v>0.53692484417121944</v>
@@ -892,7 +892,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K7" s="2">
-        <v>1.139248376871669</v>
+        <v>1.1392483768716679</v>
       </c>
       <c r="L7" s="2">
         <v>0.53692484417121944</v>
@@ -951,7 +951,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K8" s="2">
-        <v>-0.20365209942284179</v>
+        <v>-0.20365209942284171</v>
       </c>
       <c r="L8" s="2">
         <v>0.53692484417121944</v>
@@ -1010,7 +1010,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K9" s="2">
-        <v>0.1316857934465484</v>
+        <v>0.13168579344654871</v>
       </c>
       <c r="L9" s="2">
         <v>0.53692484417121944</v>
@@ -1128,7 +1128,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K11" s="2">
-        <v>-0.13859809711099669</v>
+        <v>-0.13859809711099691</v>
       </c>
       <c r="L11" s="2">
         <v>0.53692484417121944</v>
@@ -1187,7 +1187,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K12" s="2">
-        <v>-0.30665426974992921</v>
+        <v>-0.30665426974992932</v>
       </c>
       <c r="L12" s="2">
         <v>0.53692484417121944</v>
@@ -1246,7 +1246,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K13" s="2">
-        <v>0.64824554989893501</v>
+        <v>0.64824554989893513</v>
       </c>
       <c r="L13" s="2">
         <v>0.53692484417121944</v>
@@ -1305,7 +1305,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K14" s="2">
-        <v>-0.30665426974992921</v>
+        <v>-0.30665426974992932</v>
       </c>
       <c r="L14" s="2">
         <v>0.53692484417121944</v>
@@ -1364,7 +1364,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K15" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L15" s="2">
         <v>-1.8624580532189181</v>
@@ -1423,7 +1423,7 @@
         <v>3.9506614681192169</v>
       </c>
       <c r="K16" s="2">
-        <v>0.57080030905150081</v>
+        <v>0.57080030905150092</v>
       </c>
       <c r="L16" s="2">
         <v>0.53692484417121944</v>
@@ -1600,7 +1600,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K19" s="2">
-        <v>0.30129087090242979</v>
+        <v>0.30129087090242967</v>
       </c>
       <c r="L19" s="2">
         <v>0.53692484417121944</v>
@@ -1659,7 +1659,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K20" s="2">
-        <v>0.33846458650919797</v>
+        <v>0.33846458650919808</v>
       </c>
       <c r="L20" s="2">
         <v>-1.8624580532189181</v>
@@ -1836,7 +1836,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K23" s="2">
-        <v>-6.11528562635624E-2</v>
+        <v>-6.1152856263562677E-2</v>
       </c>
       <c r="L23" s="2">
         <v>0.53692484417121944</v>
@@ -1895,7 +1895,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K24" s="2">
-        <v>8.0571934487242092E-2</v>
+        <v>8.0571934487242022E-2</v>
       </c>
       <c r="L24" s="2">
         <v>0.53692484417121944</v>
@@ -2013,7 +2013,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K26" s="2">
-        <v>-0.64199216261931946</v>
+        <v>-0.64199216261931968</v>
       </c>
       <c r="L26" s="2">
         <v>0.53692484417121944</v>
@@ -2131,7 +2131,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K28" s="2">
-        <v>0.52975433140236061</v>
+        <v>0.52975433140236072</v>
       </c>
       <c r="L28" s="2">
         <v>-1.8624580532189181</v>
@@ -2190,7 +2190,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K29" s="2">
-        <v>0.1270390789957028</v>
+        <v>0.12703907899570249</v>
       </c>
       <c r="L29" s="2">
         <v>0.53692484417121944</v>
@@ -2249,7 +2249,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K30" s="2">
-        <v>-0.24237471984655889</v>
+        <v>-0.24237471984655881</v>
       </c>
       <c r="L30" s="2">
         <v>-1.8624580532189181</v>
@@ -2367,7 +2367,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K32" s="2">
-        <v>0.7311119576056897</v>
+        <v>0.73111195760568981</v>
       </c>
       <c r="L32" s="2">
         <v>0.53692484417121944</v>
@@ -2426,7 +2426,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K33" s="2">
-        <v>0.64282438303961464</v>
+        <v>0.64282438303961476</v>
       </c>
       <c r="L33" s="2">
         <v>0.53692484417121944</v>
@@ -2485,7 +2485,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K34" s="2">
-        <v>0.73343531483111291</v>
+        <v>0.73343531483111279</v>
       </c>
       <c r="L34" s="2">
         <v>-1.8624580532189181</v>
@@ -2603,7 +2603,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K36" s="2">
-        <v>0.20913103429398269</v>
+        <v>0.20913103429398289</v>
       </c>
       <c r="L36" s="2">
         <v>0.53692484417121944</v>
@@ -2721,7 +2721,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K38" s="2">
-        <v>0.98126008554290223</v>
+        <v>0.98126008554290245</v>
       </c>
       <c r="L38" s="2">
         <v>-1.8624580532189181</v>
@@ -2780,7 +2780,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K39" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L39" s="2">
         <v>0.53692484417121944</v>
@@ -2898,7 +2898,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K41" s="2">
-        <v>0.36479596839732598</v>
+        <v>0.36479596839732581</v>
       </c>
       <c r="L41" s="2">
         <v>0.53692484417121944</v>
@@ -2957,7 +2957,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K42" s="2">
-        <v>0.3098098473956476</v>
+        <v>0.30980984739564738</v>
       </c>
       <c r="L42" s="2">
         <v>-1.8624580532189181</v>
@@ -3016,7 +3016,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K43" s="2">
-        <v>0.20913103429398269</v>
+        <v>0.20913103429398289</v>
       </c>
       <c r="L43" s="2">
         <v>-1.8624580532189181</v>
@@ -3075,7 +3075,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K44" s="2">
-        <v>0.21997336801262379</v>
+        <v>0.21997336801262371</v>
       </c>
       <c r="L44" s="2">
         <v>0.53692484417121944</v>
@@ -3193,7 +3193,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K46" s="2">
-        <v>0.71252509980230527</v>
+        <v>0.71252509980230561</v>
       </c>
       <c r="L46" s="2">
         <v>0.53692484417121944</v>
@@ -3252,7 +3252,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K47" s="2">
-        <v>-0.31904550828551842</v>
+        <v>-0.31904550828551881</v>
       </c>
       <c r="L47" s="2">
         <v>0.53692484417121944</v>
@@ -3429,7 +3429,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K50" s="2">
-        <v>5.5015005007588921E-2</v>
+        <v>5.5015005007588713E-2</v>
       </c>
       <c r="L50" s="2">
         <v>0.53692484417121944</v>
@@ -3488,7 +3488,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K51" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L51" s="2">
         <v>0.53692484417121944</v>
@@ -3547,7 +3547,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K52" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L52" s="2">
         <v>0.53692484417121944</v>
@@ -3606,7 +3606,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K53" s="2">
-        <v>-5.9603951446614102E-2</v>
+        <v>-5.9603951446613963E-2</v>
       </c>
       <c r="L53" s="2">
         <v>-1.8624580532189181</v>
@@ -3665,7 +3665,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K54" s="2">
-        <v>-0.46154475144479767</v>
+        <v>-0.46154475144479779</v>
       </c>
       <c r="L54" s="2">
         <v>0.53692484417121944</v>
@@ -3724,7 +3724,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K55" s="2">
-        <v>-0.13859809711099669</v>
+        <v>-0.13859809711099691</v>
       </c>
       <c r="L55" s="2">
         <v>0.53692484417121944</v>
@@ -3783,7 +3783,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K56" s="2">
-        <v>0.24862810712617461</v>
+        <v>0.24862810712617439</v>
       </c>
       <c r="L56" s="2">
         <v>0.53692484417121944</v>
@@ -4019,7 +4019,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K60" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L60" s="2">
         <v>0.53692484417121944</v>
@@ -4078,7 +4078,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K61" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L61" s="2">
         <v>-1.8624580532189181</v>
@@ -4196,7 +4196,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K63" s="2">
-        <v>-0.45225132254310602</v>
+        <v>-0.45225132254310568</v>
       </c>
       <c r="L63" s="2">
         <v>0.53692484417121944</v>
@@ -4255,7 +4255,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K64" s="2">
-        <v>-0.5095608007702066</v>
+        <v>-0.50956080077020693</v>
       </c>
       <c r="L64" s="2">
         <v>0.53692484417121944</v>
@@ -4432,7 +4432,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K67" s="2">
-        <v>0.33846458650919797</v>
+        <v>0.33846458650919808</v>
       </c>
       <c r="L67" s="2">
         <v>0.53692484417121944</v>
@@ -4609,7 +4609,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K70" s="2">
-        <v>0.42907551830069629</v>
+        <v>0.42907551830069618</v>
       </c>
       <c r="L70" s="2">
         <v>0.53692484417121944</v>
@@ -4668,7 +4668,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K71" s="2">
-        <v>-0.35854258111771031</v>
+        <v>-0.3585425811177102</v>
       </c>
       <c r="L71" s="2">
         <v>0.53692484417121944</v>
@@ -4727,7 +4727,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K72" s="2">
-        <v>0.6358543113633458</v>
+        <v>0.63585431136334569</v>
       </c>
       <c r="L72" s="2">
         <v>0.53692484417121944</v>
@@ -4904,7 +4904,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K75" s="2">
-        <v>-0.24392362466350731</v>
+        <v>-0.2439236246635075</v>
       </c>
       <c r="L75" s="2">
         <v>-1.8624580532189181</v>
@@ -5081,7 +5081,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K78" s="2">
-        <v>0.29277189440921209</v>
+        <v>0.29277189440921192</v>
       </c>
       <c r="L78" s="2">
         <v>0.53692484417121944</v>
@@ -5199,7 +5199,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K80" s="2">
-        <v>0.74660100577517674</v>
+        <v>0.74660100577517663</v>
       </c>
       <c r="L80" s="2">
         <v>0.53692484417121944</v>
@@ -5317,7 +5317,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K82" s="2">
-        <v>-3.068925627986707E-3</v>
+        <v>-3.068925627986982E-3</v>
       </c>
       <c r="L82" s="2">
         <v>0.53692484417121944</v>
@@ -5376,7 +5376,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K83" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L83" s="2">
         <v>0.53692484417121944</v>
@@ -5435,7 +5435,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K84" s="2">
-        <v>0.28735072754989172</v>
+        <v>0.28735072754989149</v>
       </c>
       <c r="L84" s="2">
         <v>0.53692484417121944</v>
@@ -5553,7 +5553,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K86" s="2">
-        <v>1.0718710173343999</v>
+        <v>1.071871017334401</v>
       </c>
       <c r="L86" s="2">
         <v>0.53692484417121944</v>
@@ -5612,7 +5612,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K87" s="2">
-        <v>0.64824554989893501</v>
+        <v>0.64824554989893513</v>
       </c>
       <c r="L87" s="2">
         <v>0.53692484417121944</v>
@@ -5671,7 +5671,7 @@
         <v>3.9506614681192169</v>
       </c>
       <c r="K88" s="2">
-        <v>0.59171052408030833</v>
+        <v>0.59171052408030811</v>
       </c>
       <c r="L88" s="2">
         <v>0.53692484417121944</v>
@@ -5730,7 +5730,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K89" s="2">
-        <v>0.40351858882104308</v>
+        <v>0.40351858882104291</v>
       </c>
       <c r="L89" s="2">
         <v>0.53692484417121944</v>
@@ -5789,7 +5789,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K90" s="2">
-        <v>0.64824554989893501</v>
+        <v>0.64824554989893513</v>
       </c>
       <c r="L90" s="2">
         <v>0.53692484417121944</v>
@@ -5848,7 +5848,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K91" s="2">
-        <v>-0.43598782196514457</v>
+        <v>-0.43598782196514452</v>
       </c>
       <c r="L91" s="2">
         <v>0.53692484417121944</v>
@@ -5966,7 +5966,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K93" s="2">
-        <v>0.41126311290578671</v>
+        <v>0.41126311290578632</v>
       </c>
       <c r="L93" s="2">
         <v>0.53692484417121944</v>
@@ -6025,7 +6025,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K94" s="2">
-        <v>0.35163027745326197</v>
+        <v>0.35163027745326192</v>
       </c>
       <c r="L94" s="2">
         <v>0.53692484417121944</v>
@@ -6084,7 +6084,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K95" s="2">
-        <v>0.24862810712617461</v>
+        <v>0.24862810712617439</v>
       </c>
       <c r="L95" s="2">
         <v>-1.8624580532189181</v>
@@ -6143,7 +6143,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K96" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L96" s="2">
         <v>0.53692484417121944</v>
@@ -6202,7 +6202,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K97" s="2">
-        <v>-0.14401926397031711</v>
+        <v>-0.14401926397031739</v>
       </c>
       <c r="L97" s="2">
         <v>0.53692484417121944</v>
@@ -6261,7 +6261,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K98" s="2">
-        <v>2.868362311946094E-2</v>
+        <v>2.8683623119461071E-2</v>
       </c>
       <c r="L98" s="2">
         <v>0.53692484417121944</v>
@@ -6320,7 +6320,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K99" s="2">
-        <v>0.68696817032265212</v>
+        <v>0.68696817032265234</v>
       </c>
       <c r="L99" s="2">
         <v>0.53692484417121944</v>
@@ -6379,7 +6379,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K100" s="2">
-        <v>0.19673979575839351</v>
+        <v>0.1967397957583934</v>
       </c>
       <c r="L100" s="2">
         <v>0.53692484417121944</v>
@@ -6438,7 +6438,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K101" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L101" s="2">
         <v>0.53692484417121944</v>
@@ -6497,7 +6497,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K102" s="2">
-        <v>-0.28109734027027611</v>
+        <v>-0.28109734027027589</v>
       </c>
       <c r="L102" s="2">
         <v>0.53692484417121944</v>
@@ -6615,7 +6615,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K104" s="2">
-        <v>-0.66290237764812676</v>
+        <v>-0.66290237764812687</v>
       </c>
       <c r="L104" s="2">
         <v>0.53692484417121944</v>
@@ -6674,7 +6674,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K105" s="2">
-        <v>-0.74576878535488167</v>
+        <v>-0.74576878535488156</v>
       </c>
       <c r="L105" s="2">
         <v>0.53692484417121944</v>
@@ -6733,7 +6733,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K106" s="2">
-        <v>0.5971316909396287</v>
+        <v>0.59713169093962859</v>
       </c>
       <c r="L106" s="2">
         <v>0.53692484417121944</v>
@@ -6851,7 +6851,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K108" s="2">
-        <v>-0.63657099575999909</v>
+        <v>-0.6365709957599992</v>
       </c>
       <c r="L108" s="2">
         <v>0.53692484417121944</v>
@@ -7087,7 +7087,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K112" s="2">
-        <v>0.36479596839732598</v>
+        <v>0.36479596839732581</v>
       </c>
       <c r="L112" s="2">
         <v>0.53692484417121944</v>
@@ -7205,7 +7205,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K114" s="2">
-        <v>-4.8761617727973321E-2</v>
+        <v>-4.8761617727973182E-2</v>
       </c>
       <c r="L114" s="2">
         <v>0.53692484417121944</v>
@@ -7264,7 +7264,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K115" s="2">
-        <v>-0.37093381965329952</v>
+        <v>-0.37093381965329969</v>
       </c>
       <c r="L115" s="2">
         <v>0.53692484417121944</v>
@@ -7323,7 +7323,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K116" s="2">
-        <v>-0.31981996069399321</v>
+        <v>-0.3198199606939931</v>
       </c>
       <c r="L116" s="2">
         <v>0.53692484417121944</v>
@@ -7382,7 +7382,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K117" s="2">
-        <v>5.4240552599114179E-2</v>
+        <v>5.4240552599114387E-2</v>
       </c>
       <c r="L117" s="2">
         <v>0.53692484417121944</v>
@@ -7441,7 +7441,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K118" s="2">
-        <v>-0.20365209942284179</v>
+        <v>-0.20365209942284171</v>
       </c>
       <c r="L118" s="2">
         <v>-1.8624580532189181</v>
@@ -7500,7 +7500,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K119" s="2">
-        <v>-0.22920902890249489</v>
+        <v>-0.229209028902495</v>
       </c>
       <c r="L119" s="2">
         <v>0.53692484417121944</v>
@@ -7559,7 +7559,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K120" s="2">
-        <v>0.63043314450402543</v>
+        <v>0.63043314450402521</v>
       </c>
       <c r="L120" s="2">
         <v>0.53692484417121944</v>
@@ -7618,7 +7618,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K121" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L121" s="2">
         <v>-1.8624580532189181</v>
@@ -7795,7 +7795,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K124" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L124" s="2">
         <v>-1.8624580532189181</v>
@@ -7913,7 +7913,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K126" s="2">
-        <v>-6.16673526188408E-3</v>
+        <v>-6.1667352618843549E-3</v>
       </c>
       <c r="L126" s="2">
         <v>0.53692484417121944</v>
@@ -8031,7 +8031,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K128" s="2">
-        <v>0.56305578496675734</v>
+        <v>0.56305578496675746</v>
       </c>
       <c r="L128" s="2">
         <v>0.53692484417121944</v>
@@ -8149,7 +8149,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K130" s="2">
-        <v>-3.20310627744397</v>
+        <v>-3.2031062774439709</v>
       </c>
       <c r="L130" s="2">
         <v>0.53692484417121944</v>
@@ -8208,7 +8208,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K131" s="2">
-        <v>-3.5595926783909299E-2</v>
+        <v>-3.5595926783909368E-2</v>
       </c>
       <c r="L131" s="2">
         <v>0.53692484417121944</v>
@@ -8267,7 +8267,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K132" s="2">
-        <v>0.3570514443125824</v>
+        <v>0.35705144431258229</v>
       </c>
       <c r="L132" s="2">
         <v>0.53692484417121944</v>
@@ -8326,7 +8326,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K133" s="2">
-        <v>0.13478360308044629</v>
+        <v>0.13478360308044601</v>
       </c>
       <c r="L133" s="2">
         <v>0.53692484417121944</v>
@@ -8385,7 +8385,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K134" s="2">
-        <v>0.61726745355996149</v>
+        <v>0.61726745355996138</v>
       </c>
       <c r="L134" s="2">
         <v>-1.8624580532189181</v>
@@ -8444,7 +8444,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K135" s="2">
-        <v>-0.74576878535488167</v>
+        <v>-0.74576878535488156</v>
       </c>
       <c r="L135" s="2">
         <v>0.53692484417121944</v>
@@ -8739,7 +8739,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K140" s="2">
-        <v>2.171355144319221E-2</v>
+        <v>2.1713551443192002E-2</v>
       </c>
       <c r="L140" s="2">
         <v>-1.8624580532189181</v>
@@ -8857,7 +8857,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K142" s="2">
-        <v>0.72104407629552358</v>
+        <v>0.72104407629552336</v>
       </c>
       <c r="L142" s="2">
         <v>0.53692484417121944</v>
@@ -8916,7 +8916,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K143" s="2">
-        <v>0.72569079074636933</v>
+        <v>0.72569079074636944</v>
       </c>
       <c r="L143" s="2">
         <v>0.53692484417121944</v>
@@ -8975,7 +8975,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K144" s="2">
-        <v>-0.49019949055834883</v>
+        <v>-0.49019949055834838</v>
       </c>
       <c r="L144" s="2">
         <v>-1.8624580532189181</v>
@@ -9034,7 +9034,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K145" s="2">
-        <v>2.868362311946094E-2</v>
+        <v>2.8683623119461071E-2</v>
       </c>
       <c r="L145" s="2">
         <v>0.53692484417121944</v>
@@ -9093,7 +9093,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K146" s="2">
-        <v>1.139248376871669</v>
+        <v>1.1392483768716679</v>
       </c>
       <c r="L146" s="2">
         <v>0.53692484417121944</v>
@@ -9211,7 +9211,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K148" s="2">
-        <v>-0.19048640847877779</v>
+        <v>-0.1904864084787779</v>
       </c>
       <c r="L148" s="2">
         <v>0.53692484417121944</v>
@@ -9270,7 +9270,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K149" s="2">
-        <v>9.3737625431306051E-2</v>
+        <v>9.3737625431305843E-2</v>
       </c>
       <c r="L149" s="2">
         <v>0.53692484417121944</v>
@@ -9388,7 +9388,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K151" s="2">
-        <v>4.1849314063524962E-2</v>
+        <v>4.1849314063524892E-2</v>
       </c>
       <c r="L151" s="2">
         <v>-1.8624580532189181</v>
@@ -9447,7 +9447,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K152" s="2">
-        <v>0.72026962388704885</v>
+        <v>0.72026962388704896</v>
       </c>
       <c r="L152" s="2">
         <v>0.53692484417121944</v>
@@ -9506,7 +9506,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K153" s="2">
-        <v>0.42907551830069629</v>
+        <v>0.42907551830069618</v>
       </c>
       <c r="L153" s="2">
         <v>0.53692484417121944</v>
@@ -9683,7 +9683,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K156" s="2">
-        <v>0.33846458650919797</v>
+        <v>0.33846458650919808</v>
       </c>
       <c r="L156" s="2">
         <v>0.53692484417121944</v>
@@ -9801,7 +9801,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K158" s="2">
-        <v>0.54524337957184765</v>
+        <v>0.54524337957184754</v>
       </c>
       <c r="L158" s="2">
         <v>0.53692484417121944</v>
@@ -9919,7 +9919,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K160" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L160" s="2">
         <v>0.53692484417121944</v>
@@ -9978,7 +9978,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K161" s="2">
-        <v>-0.39958855876685068</v>
+        <v>-0.39958855876685029</v>
       </c>
       <c r="L161" s="2">
         <v>-1.8624580532189181</v>
@@ -10037,7 +10037,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K162" s="2">
-        <v>0.44224120924476018</v>
+        <v>0.44224120924476001</v>
       </c>
       <c r="L162" s="2">
         <v>0.53692484417121944</v>
@@ -10214,7 +10214,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K165" s="2">
-        <v>-0.41507760693633722</v>
+        <v>-0.41507760693633727</v>
       </c>
       <c r="L165" s="2">
         <v>0.53692484417121944</v>
@@ -10332,7 +10332,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K167" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L167" s="2">
         <v>0.53692484417121944</v>
@@ -10391,7 +10391,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K168" s="2">
-        <v>-7.1995189982203306E-2</v>
+        <v>-7.1995189982203445E-2</v>
       </c>
       <c r="L168" s="2">
         <v>-1.8624580532189181</v>
@@ -10450,7 +10450,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K169" s="2">
-        <v>0.1603405325600995</v>
+        <v>0.16034053256009931</v>
       </c>
       <c r="L169" s="2">
         <v>0.53692484417121944</v>
@@ -10509,7 +10509,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K170" s="2">
-        <v>-0.24237471984655889</v>
+        <v>-0.24237471984655881</v>
       </c>
       <c r="L170" s="2">
         <v>0.53692484417121944</v>
@@ -10568,7 +10568,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K171" s="2">
-        <v>0.76441341117008643</v>
+        <v>0.76441341117008654</v>
       </c>
       <c r="L171" s="2">
         <v>0.53692484417121944</v>
@@ -10627,7 +10627,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K172" s="2">
-        <v>-0.28032288786180132</v>
+        <v>-0.28032288786180171</v>
       </c>
       <c r="L172" s="2">
         <v>0.53692484417121944</v>
@@ -10745,7 +10745,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K174" s="2">
-        <v>-0.47471044238886168</v>
+        <v>-0.47471044238886162</v>
       </c>
       <c r="L174" s="2">
         <v>0.53692484417121944</v>
@@ -10863,7 +10863,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K176" s="2">
-        <v>0.59325942889725669</v>
+        <v>0.5932594288972568</v>
       </c>
       <c r="L176" s="2">
         <v>0.53692484417121944</v>
@@ -10922,7 +10922,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K177" s="2">
-        <v>0.42133099421595271</v>
+        <v>0.42133099421595283</v>
       </c>
       <c r="L177" s="2">
         <v>0.53692484417121944</v>
@@ -11040,7 +11040,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K179" s="2">
-        <v>0.3570514443125824</v>
+        <v>0.35705144431258229</v>
       </c>
       <c r="L179" s="2">
         <v>0.53692484417121944</v>
@@ -11158,7 +11158,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K181" s="2">
-        <v>0.41590982735663229</v>
+        <v>0.4159098273566324</v>
       </c>
       <c r="L181" s="2">
         <v>0.53692484417121944</v>
@@ -11217,7 +11217,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K182" s="2">
-        <v>0.35937480153800561</v>
+        <v>0.35937480153800527</v>
       </c>
       <c r="L182" s="2">
         <v>0.53692484417121944</v>
@@ -11335,7 +11335,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K184" s="2">
-        <v>0.24862810712617461</v>
+        <v>0.24862810712617439</v>
       </c>
       <c r="L184" s="2">
         <v>-1.8624580532189181</v>
@@ -11394,7 +11394,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K185" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L185" s="2">
         <v>0.53692484417121944</v>
@@ -11453,7 +11453,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K186" s="2">
-        <v>7.5150767627921666E-2</v>
+        <v>7.5150767627921611E-2</v>
       </c>
       <c r="L186" s="2">
         <v>0.53692484417121944</v>
@@ -11512,7 +11512,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K187" s="2">
-        <v>1.6292384583871861E-2</v>
+        <v>1.629238458387158E-2</v>
       </c>
       <c r="L187" s="2">
         <v>-1.8624580532189181</v>
@@ -11630,7 +11630,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K189" s="2">
-        <v>-0.35079805703296668</v>
+        <v>-0.35079805703296679</v>
       </c>
       <c r="L189" s="2">
         <v>0.53692484417121944</v>
@@ -11689,7 +11689,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K190" s="2">
-        <v>0.45463244778034939</v>
+        <v>0.4546324477803495</v>
       </c>
       <c r="L190" s="2">
         <v>0.53692484417121944</v>
@@ -11748,7 +11748,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K191" s="2">
-        <v>-7.4318547207626429E-2</v>
+        <v>-7.4318547207626498E-2</v>
       </c>
       <c r="L191" s="2">
         <v>-1.8624580532189181</v>
@@ -11984,7 +11984,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K195" s="2">
-        <v>0.44224120924476018</v>
+        <v>0.44224120924476001</v>
       </c>
       <c r="L195" s="2">
         <v>0.53692484417121944</v>
@@ -12102,7 +12102,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K197" s="2">
-        <v>-7.1995189982203306E-2</v>
+        <v>-7.1995189982203445E-2</v>
       </c>
       <c r="L197" s="2">
         <v>0.53692484417121944</v>
@@ -12161,7 +12161,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K198" s="2">
-        <v>-0.26793164932621211</v>
+        <v>-0.26793164932621222</v>
       </c>
       <c r="L198" s="2">
         <v>0.53692484417121944</v>
@@ -12220,7 +12220,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K199" s="2">
-        <v>0.80313603159380353</v>
+        <v>0.80313603159380365</v>
       </c>
       <c r="L199" s="2">
         <v>-1.8624580532189181</v>
@@ -12279,7 +12279,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K200" s="2">
-        <v>0.79074479305821432</v>
+        <v>0.79074479305821421</v>
       </c>
       <c r="L200" s="2">
         <v>0.53692484417121944</v>
@@ -12397,7 +12397,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K202" s="2">
-        <v>-0.24469807707198199</v>
+        <v>-0.2446980770719818</v>
       </c>
       <c r="L202" s="2">
         <v>0.53692484417121944</v>
@@ -12456,7 +12456,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K203" s="2">
-        <v>0.40351858882104308</v>
+        <v>0.40351858882104291</v>
       </c>
       <c r="L203" s="2">
         <v>-1.8624580532189181</v>
@@ -12515,7 +12515,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K204" s="2">
-        <v>8.9865363388934E-2</v>
+        <v>8.9865363388934139E-2</v>
       </c>
       <c r="L204" s="2">
         <v>0.53692484417121944</v>
@@ -12574,7 +12574,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K205" s="2">
-        <v>-0.75816002389047088</v>
+        <v>-0.75816002389047099</v>
       </c>
       <c r="L205" s="2">
         <v>0.53692484417121944</v>
@@ -12633,7 +12633,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K206" s="2">
-        <v>0.42907551830069629</v>
+        <v>0.42907551830069618</v>
       </c>
       <c r="L206" s="2">
         <v>0.53692484417121944</v>
@@ -12692,7 +12692,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K207" s="2">
-        <v>0.77525574488872728</v>
+        <v>0.77525574488872739</v>
       </c>
       <c r="L207" s="2">
         <v>-1.8624580532189181</v>
@@ -12810,7 +12810,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K209" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L209" s="2">
         <v>0.53692484417121944</v>
@@ -12869,7 +12869,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K210" s="2">
-        <v>-0.17112509826691921</v>
+        <v>-0.1711250982669193</v>
       </c>
       <c r="L210" s="2">
         <v>0.53692484417121944</v>
@@ -12987,7 +12987,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K212" s="2">
-        <v>0.87516010558191737</v>
+        <v>0.87516010558191748</v>
       </c>
       <c r="L212" s="2">
         <v>0.53692484417121944</v>
@@ -13105,7 +13105,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K214" s="2">
-        <v>1.6292384583871861E-2</v>
+        <v>1.629238458387158E-2</v>
       </c>
       <c r="L214" s="2">
         <v>0.53692484417121944</v>
@@ -13164,7 +13164,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K215" s="2">
-        <v>-0.4406345364159901</v>
+        <v>-0.4406345364159906</v>
       </c>
       <c r="L215" s="2">
         <v>0.53692484417121944</v>
@@ -13223,7 +13223,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K216" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L216" s="2">
         <v>0.53692484417121944</v>
@@ -13282,7 +13282,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K217" s="2">
-        <v>0.4801893772600026</v>
+        <v>0.48018937726000283</v>
       </c>
       <c r="L217" s="2">
         <v>0.53692484417121944</v>
@@ -13341,7 +13341,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K218" s="2">
-        <v>0.44224120924476018</v>
+        <v>0.44224120924476001</v>
       </c>
       <c r="L218" s="2">
         <v>-1.8624580532189181</v>
@@ -13400,7 +13400,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K219" s="2">
-        <v>-0.53898999229223199</v>
+        <v>-0.5389899922922321</v>
       </c>
       <c r="L219" s="2">
         <v>0.53692484417121944</v>
@@ -13636,7 +13636,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K223" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L223" s="2">
         <v>0.53692484417121944</v>
@@ -13813,7 +13813,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K226" s="2">
-        <v>0.71794626666162575</v>
+        <v>0.71794626666162598</v>
       </c>
       <c r="L226" s="2">
         <v>0.53692484417121944</v>
@@ -13990,7 +13990,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K229" s="2">
-        <v>0.66915576492774198</v>
+        <v>0.66915576492774242</v>
       </c>
       <c r="L229" s="2">
         <v>-1.8624580532189181</v>
@@ -14108,7 +14108,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K231" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L231" s="2">
         <v>-1.8624580532189181</v>
@@ -14167,7 +14167,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K232" s="2">
-        <v>-7.1995189982203306E-2</v>
+        <v>-7.1995189982203445E-2</v>
       </c>
       <c r="L232" s="2">
         <v>0.53692484417121944</v>
@@ -14403,7 +14403,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K236" s="2">
-        <v>-7.9739714066946854E-2</v>
+        <v>-7.973971406694691E-2</v>
       </c>
       <c r="L236" s="2">
         <v>0.53692484417121944</v>
@@ -14462,7 +14462,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K237" s="2">
-        <v>0.57080030905150081</v>
+        <v>0.57080030905150092</v>
       </c>
       <c r="L237" s="2">
         <v>0.53692484417121944</v>
@@ -14580,7 +14580,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K239" s="2">
-        <v>-0.25863822042452028</v>
+        <v>-0.25863822042452012</v>
       </c>
       <c r="L239" s="2">
         <v>0.53692484417121944</v>
@@ -14698,7 +14698,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K241" s="2">
-        <v>0.42133099421595271</v>
+        <v>0.42133099421595283</v>
       </c>
       <c r="L241" s="2">
         <v>0.53692484417121944</v>
@@ -14757,7 +14757,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K242" s="2">
-        <v>-0.57771261271594909</v>
+        <v>-0.5777126127159492</v>
       </c>
       <c r="L242" s="2">
         <v>0.53692484417121944</v>
@@ -14816,7 +14816,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K243" s="2">
-        <v>-0.1285302158008306</v>
+        <v>-0.12853021580083049</v>
       </c>
       <c r="L243" s="2">
         <v>0.53692484417121944</v>
@@ -14875,7 +14875,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K244" s="2">
-        <v>0.49335506820406649</v>
+        <v>0.49335506820406672</v>
       </c>
       <c r="L244" s="2">
         <v>0.53692484417121944</v>
@@ -15111,7 +15111,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K248" s="2">
-        <v>0.77525574488872728</v>
+        <v>0.77525574488872739</v>
       </c>
       <c r="L248" s="2">
         <v>0.53692484417121944</v>
@@ -15170,7 +15170,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K249" s="2">
-        <v>7.5150767627921666E-2</v>
+        <v>7.5150767627921611E-2</v>
       </c>
       <c r="L249" s="2">
         <v>0.53692484417121944</v>
@@ -15288,7 +15288,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K251" s="2">
-        <v>-0.46154475144479767</v>
+        <v>-0.46154475144479779</v>
       </c>
       <c r="L251" s="2">
         <v>0.53692484417121944</v>
@@ -15406,7 +15406,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K253" s="2">
-        <v>-0.37093381965329952</v>
+        <v>-0.37093381965329969</v>
       </c>
       <c r="L253" s="2">
         <v>-1.8624580532189181</v>
@@ -15465,7 +15465,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K254" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L254" s="2">
         <v>0.53692484417121944</v>
@@ -15524,7 +15524,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K255" s="2">
-        <v>-4.7987165319498593E-2</v>
+        <v>-4.7987165319498863E-2</v>
       </c>
       <c r="L255" s="2">
         <v>0.53692484417121944</v>
@@ -15642,7 +15642,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K257" s="2">
-        <v>-0.16415502659065001</v>
+        <v>-0.16415502659065029</v>
       </c>
       <c r="L257" s="2">
         <v>0.53692484417121944</v>
@@ -15760,7 +15760,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K259" s="2">
-        <v>0.67922364623790865</v>
+        <v>0.67922364623790887</v>
       </c>
       <c r="L259" s="2">
         <v>0.53692484417121944</v>
@@ -15819,7 +15819,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K260" s="2">
-        <v>-1.0346395337158121</v>
+        <v>-1.034639533715811</v>
       </c>
       <c r="L260" s="2">
         <v>0.53692484417121944</v>
@@ -15878,7 +15878,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K261" s="2">
-        <v>0.1711828662787403</v>
+        <v>0.1711828662787401</v>
       </c>
       <c r="L261" s="2">
         <v>-1.8624580532189181</v>
@@ -15937,7 +15937,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K262" s="2">
-        <v>1.3274403121309339</v>
+        <v>1.3274403121309331</v>
       </c>
       <c r="L262" s="2">
         <v>-1.8624580532189181</v>
@@ -16055,7 +16055,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K264" s="2">
-        <v>0.98435789517680006</v>
+        <v>0.98435789517679984</v>
       </c>
       <c r="L264" s="2">
         <v>0.53692484417121944</v>
@@ -16114,7 +16114,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K265" s="2">
-        <v>0.2099054867024574</v>
+        <v>0.20990548670245721</v>
       </c>
       <c r="L265" s="2">
         <v>0.53692484417121944</v>
@@ -16173,7 +16173,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K266" s="2">
-        <v>-0.26793164932621211</v>
+        <v>-0.26793164932621222</v>
       </c>
       <c r="L266" s="2">
         <v>0.53692484417121944</v>
@@ -16232,7 +16232,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K267" s="2">
-        <v>0.14794929402451021</v>
+        <v>0.14794929402450979</v>
       </c>
       <c r="L267" s="2">
         <v>0.53692484417121944</v>
@@ -16291,7 +16291,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K268" s="2">
-        <v>0.49335506820406649</v>
+        <v>0.49335506820406672</v>
       </c>
       <c r="L268" s="2">
         <v>0.53692484417121944</v>
@@ -16586,7 +16586,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K273" s="2">
-        <v>0.80313603159380353</v>
+        <v>0.80313603159380365</v>
       </c>
       <c r="L273" s="2">
         <v>0.53692484417121944</v>
@@ -16645,7 +16645,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K274" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L274" s="2">
         <v>0.53692484417121944</v>
@@ -16704,7 +16704,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K275" s="2">
-        <v>-0.4135287021193888</v>
+        <v>-0.41352870211938858</v>
       </c>
       <c r="L275" s="2">
         <v>0.53692484417121944</v>
@@ -16763,7 +16763,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K276" s="2">
-        <v>-0.14944043082963759</v>
+        <v>-0.1494404308296377</v>
       </c>
       <c r="L276" s="2">
         <v>0.53692484417121944</v>
@@ -16881,7 +16881,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K278" s="2">
-        <v>-6.5025118305934521E-2</v>
+        <v>-6.5025118305934382E-2</v>
       </c>
       <c r="L278" s="2">
         <v>0.53692484417121944</v>
@@ -16940,7 +16940,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K279" s="2">
-        <v>0.30051641849395572</v>
+        <v>0.30051641849395527</v>
       </c>
       <c r="L279" s="2">
         <v>0.53692484417121944</v>
@@ -16999,7 +16999,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K280" s="2">
-        <v>8.8316458571985626E-2</v>
+        <v>8.8316458571985418E-2</v>
       </c>
       <c r="L280" s="2">
         <v>0.53692484417121944</v>
@@ -17058,7 +17058,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K281" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L281" s="2">
         <v>-1.8624580532189181</v>
@@ -17117,7 +17117,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K282" s="2">
-        <v>0.19673979575839351</v>
+        <v>0.1967397957583934</v>
       </c>
       <c r="L282" s="2">
         <v>0.53692484417121944</v>
@@ -17176,7 +17176,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K283" s="2">
-        <v>0.41590982735663229</v>
+        <v>0.4159098273566324</v>
       </c>
       <c r="L283" s="2">
         <v>0.53692484417121944</v>
@@ -17294,7 +17294,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K285" s="2">
-        <v>0.4352711375684909</v>
+        <v>0.43527113756849101</v>
       </c>
       <c r="L285" s="2">
         <v>-1.8624580532189181</v>
@@ -17353,7 +17353,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K286" s="2">
-        <v>0.35782589672105658</v>
+        <v>0.35782589672105669</v>
       </c>
       <c r="L286" s="2">
         <v>0.53692484417121944</v>
@@ -17471,7 +17471,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K288" s="2">
-        <v>0.28657627514141698</v>
+        <v>0.28657627514141709</v>
       </c>
       <c r="L288" s="2">
         <v>0.53692484417121944</v>
@@ -17530,7 +17530,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K289" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L289" s="2">
         <v>0.53692484417121944</v>
@@ -17707,7 +17707,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K292" s="2">
-        <v>-0.71943740346675378</v>
+        <v>-0.71943740346675389</v>
       </c>
       <c r="L292" s="2">
         <v>0.53692484417121944</v>
@@ -17766,7 +17766,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K293" s="2">
-        <v>-0.25476595838214811</v>
+        <v>-0.25476595838214833</v>
       </c>
       <c r="L293" s="2">
         <v>0.53692484417121944</v>
@@ -17884,7 +17884,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K295" s="2">
-        <v>4.1849314063524962E-2</v>
+        <v>4.1849314063524892E-2</v>
       </c>
       <c r="L295" s="2">
         <v>0.53692484417121944</v>
@@ -17943,7 +17943,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K296" s="2">
-        <v>0.75124772022602249</v>
+        <v>0.75124772022602271</v>
       </c>
       <c r="L296" s="2">
         <v>-1.8624580532189181</v>
@@ -18238,7 +18238,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K301" s="2">
-        <v>0.80700829363617554</v>
+        <v>0.80700829363617532</v>
       </c>
       <c r="L301" s="2">
         <v>0.53692484417121944</v>
@@ -18297,7 +18297,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K302" s="2">
-        <v>-0.26793164932621211</v>
+        <v>-0.26793164932621222</v>
       </c>
       <c r="L302" s="2">
         <v>0.53692484417121944</v>
@@ -18474,7 +18474,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K305" s="2">
-        <v>-0.41043089248549153</v>
+        <v>-0.41043089248549119</v>
       </c>
       <c r="L305" s="2">
         <v>0.53692484417121944</v>
@@ -18651,7 +18651,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K308" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L308" s="2">
         <v>0.53692484417121944</v>
@@ -18710,7 +18710,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K309" s="2">
-        <v>-2.3204688248320011E-2</v>
+        <v>-2.3204688248319869E-2</v>
       </c>
       <c r="L309" s="2">
         <v>0.53692484417121944</v>
@@ -18769,7 +18769,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K310" s="2">
-        <v>-0.1773207175347139</v>
+        <v>-0.1773207175347141</v>
       </c>
       <c r="L310" s="2">
         <v>-1.8624580532189181</v>
@@ -18946,7 +18946,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K313" s="2">
-        <v>-4.8761617727973321E-2</v>
+        <v>-4.8761617727973182E-2</v>
       </c>
       <c r="L313" s="2">
         <v>0.53692484417121944</v>
@@ -19123,7 +19123,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K316" s="2">
-        <v>-0.68071478304303668</v>
+        <v>-0.68071478304303679</v>
       </c>
       <c r="L316" s="2">
         <v>0.53692484417121944</v>
@@ -19241,7 +19241,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K318" s="2">
-        <v>0.29741860886005778</v>
+        <v>0.29741860886005789</v>
       </c>
       <c r="L318" s="2">
         <v>0.53692484417121944</v>
@@ -19300,7 +19300,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K319" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L319" s="2">
         <v>-1.8624580532189181</v>
@@ -19359,7 +19359,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K320" s="2">
-        <v>0.32607334797360882</v>
+        <v>0.32607334797360871</v>
       </c>
       <c r="L320" s="2">
         <v>-1.8624580532189181</v>
@@ -19418,7 +19418,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K321" s="2">
-        <v>-2.2430235839845269E-2</v>
+        <v>-2.243023583984555E-2</v>
       </c>
       <c r="L321" s="2">
         <v>0.53692484417121944</v>
@@ -19477,7 +19477,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K322" s="2">
-        <v>-0.66135347283117807</v>
+        <v>-0.66135347283117818</v>
       </c>
       <c r="L322" s="2">
         <v>-1.8624580532189181</v>
@@ -19595,7 +19595,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K324" s="2">
-        <v>0.41668427976510702</v>
+        <v>0.41668427976510669</v>
       </c>
       <c r="L324" s="2">
         <v>-1.8624580532189181</v>
@@ -19949,7 +19949,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K330" s="2">
-        <v>0.40274413641256829</v>
+        <v>0.40274413641256862</v>
       </c>
       <c r="L330" s="2">
         <v>0.53692484417121944</v>
@@ -20126,7 +20126,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K333" s="2">
-        <v>0.17040841387026559</v>
+        <v>0.17040841387026581</v>
       </c>
       <c r="L333" s="2">
         <v>0.53692484417121944</v>
@@ -20185,7 +20185,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K334" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L334" s="2">
         <v>0.53692484417121944</v>
@@ -20244,7 +20244,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K335" s="2">
-        <v>0.54524337957184765</v>
+        <v>0.54524337957184754</v>
       </c>
       <c r="L335" s="2">
         <v>-1.8624580532189181</v>
@@ -20362,7 +20362,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K337" s="2">
-        <v>0.35163027745326197</v>
+        <v>0.35163027745326192</v>
       </c>
       <c r="L337" s="2">
         <v>-1.8624580532189181</v>
@@ -20421,7 +20421,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K338" s="2">
-        <v>-6.11528562635624E-2</v>
+        <v>-6.1152856263562677E-2</v>
       </c>
       <c r="L338" s="2">
         <v>0.53692484417121944</v>
@@ -20480,7 +20480,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K339" s="2">
-        <v>0.43449668516001672</v>
+        <v>0.4344966851600166</v>
       </c>
       <c r="L339" s="2">
         <v>0.53692484417121944</v>
@@ -20539,7 +20539,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K340" s="2">
-        <v>1.1802943545208091</v>
+        <v>1.180294354520808</v>
       </c>
       <c r="L340" s="2">
         <v>-1.8624580532189181</v>
@@ -20598,7 +20598,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K341" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L341" s="2">
         <v>0.53692484417121944</v>
@@ -20657,7 +20657,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K342" s="2">
-        <v>0.79074479305821432</v>
+        <v>0.79074479305821421</v>
       </c>
       <c r="L342" s="2">
         <v>0.53692484417121944</v>
@@ -20716,7 +20716,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K343" s="2">
-        <v>0.71562290943620321</v>
+        <v>0.71562290943620288</v>
       </c>
       <c r="L343" s="2">
         <v>0.53692484417121944</v>
@@ -20775,7 +20775,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K344" s="2">
-        <v>0.75202217263449722</v>
+        <v>0.75202217263449711</v>
       </c>
       <c r="L344" s="2">
         <v>-1.8624580532189181</v>
@@ -20893,7 +20893,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K346" s="2">
-        <v>-7.0446285165254863E-2</v>
+        <v>-7.0446285165254793E-2</v>
       </c>
       <c r="L346" s="2">
         <v>0.53692484417121944</v>
@@ -20952,7 +20952,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K347" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L347" s="2">
         <v>-1.8624580532189181</v>
@@ -21011,7 +21011,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K348" s="2">
-        <v>-0.48710168092445089</v>
+        <v>-0.48710168092445111</v>
       </c>
       <c r="L348" s="2">
         <v>0.53692484417121944</v>
@@ -21070,7 +21070,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K349" s="2">
-        <v>0.87283674835649427</v>
+        <v>0.8728367483564945</v>
       </c>
       <c r="L349" s="2">
         <v>-1.8624580532189181</v>
@@ -21129,7 +21129,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K350" s="2">
-        <v>0.53749885548710408</v>
+        <v>0.53749885548710419</v>
       </c>
       <c r="L350" s="2">
         <v>0.53692484417121944</v>
@@ -21188,7 +21188,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K351" s="2">
-        <v>1.3661629325546509</v>
+        <v>1.36616293255465</v>
       </c>
       <c r="L351" s="2">
         <v>0.53692484417121944</v>
@@ -21247,7 +21247,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K352" s="2">
-        <v>0.40351858882104308</v>
+        <v>0.40351858882104291</v>
       </c>
       <c r="L352" s="2">
         <v>0.53692484417121944</v>
@@ -21306,7 +21306,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K353" s="2">
-        <v>0.15801717533467641</v>
+        <v>0.1580171753346763</v>
       </c>
       <c r="L353" s="2">
         <v>0.53692484417121944</v>
@@ -21365,7 +21365,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K354" s="2">
-        <v>-0.12078569171608711</v>
+        <v>-0.120785691716087</v>
       </c>
       <c r="L354" s="2">
         <v>0.53692484417121944</v>
@@ -21542,7 +21542,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K357" s="2">
-        <v>0.40351858882104308</v>
+        <v>0.40351858882104291</v>
       </c>
       <c r="L357" s="2">
         <v>0.53692484417121944</v>
@@ -21601,7 +21601,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K358" s="2">
-        <v>0.17428067591263771</v>
+        <v>0.17428067591263749</v>
       </c>
       <c r="L358" s="2">
         <v>0.53692484417121944</v>
@@ -21660,7 +21660,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K359" s="2">
-        <v>0.41668427976510702</v>
+        <v>0.41668427976510669</v>
       </c>
       <c r="L359" s="2">
         <v>0.53692484417121944</v>
@@ -21719,7 +21719,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K360" s="2">
-        <v>-2.55280454737432E-2</v>
+        <v>-2.5528045473742919E-2</v>
       </c>
       <c r="L360" s="2">
         <v>0.53692484417121944</v>
@@ -21778,7 +21778,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K361" s="2">
-        <v>0.5584090705159116</v>
+        <v>0.55840907051591138</v>
       </c>
       <c r="L361" s="2">
         <v>-1.8624580532189181</v>
@@ -21837,7 +21837,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K362" s="2">
-        <v>-0.26793164932621211</v>
+        <v>-0.26793164932621222</v>
       </c>
       <c r="L362" s="2">
         <v>0.53692484417121944</v>
@@ -21896,7 +21896,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K363" s="2">
-        <v>-6.11528562635624E-2</v>
+        <v>-6.1152856263562677E-2</v>
       </c>
       <c r="L363" s="2">
         <v>-1.8624580532189181</v>
@@ -22014,7 +22014,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K365" s="2">
-        <v>0.20061205780076499</v>
+        <v>0.2006120578007651</v>
       </c>
       <c r="L365" s="2">
         <v>-1.8624580532189181</v>
@@ -22073,7 +22073,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K366" s="2">
-        <v>0.9998469433462871</v>
+        <v>0.99984694334628677</v>
       </c>
       <c r="L366" s="2">
         <v>0.53692484417121944</v>
@@ -22191,7 +22191,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K368" s="2">
-        <v>-0.31439879383467262</v>
+        <v>-0.31439879383467267</v>
       </c>
       <c r="L368" s="2">
         <v>0.53692484417121944</v>
@@ -22250,7 +22250,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K369" s="2">
-        <v>0.44224120924476018</v>
+        <v>0.44224120924476001</v>
       </c>
       <c r="L369" s="2">
         <v>0.53692484417121944</v>
@@ -22368,7 +22368,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K371" s="2">
-        <v>-0.1780951699431885</v>
+        <v>-0.17809516994318841</v>
       </c>
       <c r="L371" s="2">
         <v>0.53692484417121944</v>
@@ -22486,7 +22486,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K373" s="2">
-        <v>0.20603322466008539</v>
+        <v>0.2060332246600855</v>
       </c>
       <c r="L373" s="2">
         <v>-1.8624580532189181</v>
@@ -22545,7 +22545,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K374" s="2">
-        <v>0.45850470982272151</v>
+        <v>0.45850470982272118</v>
       </c>
       <c r="L374" s="2">
         <v>0.53692484417121944</v>
@@ -22604,7 +22604,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K375" s="2">
-        <v>-8.2063071292369963E-2</v>
+        <v>-8.2063071292369894E-2</v>
       </c>
       <c r="L375" s="2">
         <v>-1.8624580532189181</v>
@@ -22663,7 +22663,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K376" s="2">
-        <v>0.37796165934138992</v>
+        <v>0.37796165934138959</v>
       </c>
       <c r="L376" s="2">
         <v>0.53692484417121944</v>
@@ -22781,7 +22781,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K378" s="2">
-        <v>0.61494409633453839</v>
+        <v>0.6149440963345385</v>
       </c>
       <c r="L378" s="2">
         <v>0.53692484417121944</v>
@@ -22840,7 +22840,7 @@
         <v>2.826020612231265</v>
       </c>
       <c r="K379" s="2">
-        <v>1.4490293402614061</v>
+        <v>1.449029340261405</v>
       </c>
       <c r="L379" s="2">
         <v>0.53692484417121944</v>
@@ -22958,7 +22958,7 @@
         <v>5.0753023240071693</v>
       </c>
       <c r="K381" s="2">
-        <v>0.84573091405989231</v>
+        <v>0.84573091405989242</v>
       </c>
       <c r="L381" s="2">
         <v>-1.8624580532189181</v>
@@ -23017,7 +23017,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K382" s="2">
-        <v>0.18357410481432951</v>
+        <v>0.18357410481432959</v>
       </c>
       <c r="L382" s="2">
         <v>0.53692484417121944</v>
@@ -23076,7 +23076,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K383" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L383" s="2">
         <v>-1.8624580532189181</v>
@@ -23135,7 +23135,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K384" s="2">
-        <v>0.74660100577517674</v>
+        <v>0.74660100577517663</v>
       </c>
       <c r="L384" s="2">
         <v>0.53692484417121944</v>
@@ -23253,7 +23253,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K386" s="2">
-        <v>-0.4135287021193888</v>
+        <v>-0.41352870211938858</v>
       </c>
       <c r="L386" s="2">
         <v>0.53692484417121944</v>
@@ -23312,7 +23312,7 @@
         <v>3.9506614681192169</v>
       </c>
       <c r="K387" s="2">
-        <v>0.33923903891767282</v>
+        <v>0.33923903891767238</v>
       </c>
       <c r="L387" s="2">
         <v>0.53692484417121944</v>
@@ -23371,7 +23371,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K388" s="2">
-        <v>0.19364198612449621</v>
+        <v>0.19364198612449601</v>
       </c>
       <c r="L388" s="2">
         <v>0.53692484417121944</v>
@@ -23548,7 +23548,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K391" s="2">
-        <v>-0.48787613333292579</v>
+        <v>-0.48787613333292551</v>
       </c>
       <c r="L391" s="2">
         <v>0.53692484417121944</v>
@@ -23607,7 +23607,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K392" s="2">
-        <v>0.27418503660582783</v>
+        <v>0.27418503660582771</v>
       </c>
       <c r="L392" s="2">
         <v>-1.8624580532189181</v>
@@ -23666,7 +23666,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K393" s="2">
-        <v>1.1911366882394501</v>
+        <v>1.191136688239449</v>
       </c>
       <c r="L393" s="2">
         <v>0.53692484417121944</v>
@@ -23725,7 +23725,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K394" s="2">
-        <v>-0.34305353294822349</v>
+        <v>-0.34305353294822338</v>
       </c>
       <c r="L394" s="2">
         <v>0.53692484417121944</v>
@@ -23784,7 +23784,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K395" s="2">
-        <v>-0.42282213102108063</v>
+        <v>-0.42282213102108068</v>
       </c>
       <c r="L395" s="2">
         <v>0.53692484417121944</v>
@@ -23843,7 +23843,7 @@
         <v>3.9506614681192169</v>
       </c>
       <c r="K396" s="2">
-        <v>0.73343531483111291</v>
+        <v>0.73343531483111279</v>
       </c>
       <c r="L396" s="2">
         <v>-1.8624580532189181</v>
@@ -24197,7 +24197,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K402" s="2">
-        <v>-6.1927308672037142E-2</v>
+        <v>-6.1927308672037003E-2</v>
       </c>
       <c r="L402" s="2">
         <v>-1.8624580532189181</v>
@@ -24433,7 +24433,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K406" s="2">
-        <v>-0.51343306281257883</v>
+        <v>-0.51343306281257872</v>
       </c>
       <c r="L406" s="2">
         <v>0.53692484417121944</v>
@@ -24492,7 +24492,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K407" s="2">
-        <v>-0.30433091252450639</v>
+        <v>-0.30433091252450628</v>
       </c>
       <c r="L407" s="2">
         <v>0.53692484417121944</v>
@@ -24551,7 +24551,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K408" s="2">
-        <v>-0.37867834373804299</v>
+        <v>-0.3786783437380431</v>
       </c>
       <c r="L408" s="2">
         <v>0.53692484417121944</v>
@@ -24610,7 +24610,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K409" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L409" s="2">
         <v>0.53692484417121944</v>
@@ -24669,7 +24669,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K410" s="2">
-        <v>0.84185865201752064</v>
+        <v>0.84185865201752086</v>
       </c>
       <c r="L410" s="2">
         <v>-1.8624580532189181</v>
@@ -24846,7 +24846,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K413" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L413" s="2">
         <v>-1.8624580532189181</v>
@@ -25023,7 +25023,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K416" s="2">
-        <v>0.70245721849213927</v>
+        <v>0.70245721849213905</v>
       </c>
       <c r="L416" s="2">
         <v>0.53692484417121944</v>
@@ -25141,7 +25141,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K418" s="2">
-        <v>-0.26793164932621211</v>
+        <v>-0.26793164932621222</v>
       </c>
       <c r="L418" s="2">
         <v>0.53692484417121944</v>
@@ -25318,7 +25318,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K421" s="2">
-        <v>-0.30665426974992921</v>
+        <v>-0.30665426974992932</v>
       </c>
       <c r="L421" s="2">
         <v>0.53692484417121944</v>
@@ -25436,7 +25436,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K423" s="2">
-        <v>-0.12620685857540759</v>
+        <v>-0.12620685857540739</v>
       </c>
       <c r="L423" s="2">
         <v>0.53692484417121944</v>
@@ -25495,7 +25495,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K424" s="2">
-        <v>0.75511998226839461</v>
+        <v>0.7551199822683945</v>
       </c>
       <c r="L424" s="2">
         <v>0.53692484417121944</v>
@@ -25554,7 +25554,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K425" s="2">
-        <v>0.2099054867024574</v>
+        <v>0.20990548670245721</v>
       </c>
       <c r="L425" s="2">
         <v>-1.8624580532189181</v>
@@ -25731,7 +25731,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K428" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L428" s="2">
         <v>0.53692484417121944</v>
@@ -25790,7 +25790,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K429" s="2">
-        <v>0.1115500308262157</v>
+        <v>0.1115500308262158</v>
       </c>
       <c r="L429" s="2">
         <v>0.53692484417121944</v>
@@ -26000,7 +26000,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K2" s="2">
-        <v>-0.43056665510582398</v>
+        <v>-0.43056665510582409</v>
       </c>
       <c r="L2" s="2">
         <v>-1.8624580532189181</v>
@@ -26065,7 +26065,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K3" s="2">
-        <v>0.1270390789957028</v>
+        <v>0.12703907899570249</v>
       </c>
       <c r="L3" s="2">
         <v>0.53692484417121944</v>
@@ -26130,7 +26130,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K4" s="2">
-        <v>0.91930389286495495</v>
+        <v>0.91930389286495506</v>
       </c>
       <c r="L4" s="2">
         <v>0.53692484417121944</v>
@@ -26325,7 +26325,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K7" s="2">
-        <v>0.98358344276832532</v>
+        <v>0.98358344276832554</v>
       </c>
       <c r="L7" s="2">
         <v>-1.8624580532189181</v>
@@ -26390,7 +26390,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K8" s="2">
-        <v>-0.5924272084769614</v>
+        <v>-0.59242720847696162</v>
       </c>
       <c r="L8" s="2">
         <v>0.53692484417121944</v>
@@ -26455,7 +26455,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K9" s="2">
-        <v>-0.42282213102108063</v>
+        <v>-0.42282213102108068</v>
       </c>
       <c r="L9" s="2">
         <v>0.53692484417121944</v>
@@ -26715,7 +26715,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K13" s="2">
-        <v>0.39809742196172271</v>
+        <v>0.39809742196172249</v>
       </c>
       <c r="L13" s="2">
         <v>0.53692484417121944</v>
@@ -26845,7 +26845,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K15" s="2">
-        <v>-9.2645448957814538E-3</v>
+        <v>-9.2645448957817279E-3</v>
       </c>
       <c r="L15" s="2">
         <v>0.53692484417121944</v>
@@ -26910,7 +26910,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K16" s="2">
-        <v>0.1711828662787403</v>
+        <v>0.1711828662787401</v>
       </c>
       <c r="L16" s="2">
         <v>0.53692484417121944</v>
@@ -26975,7 +26975,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K17" s="2">
-        <v>-0.1773207175347139</v>
+        <v>-0.1773207175347141</v>
       </c>
       <c r="L17" s="2">
         <v>0.53692484417121944</v>
@@ -27040,7 +27040,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K18" s="2">
-        <v>-0.61643523313966619</v>
+        <v>-0.61643523313966631</v>
       </c>
       <c r="L18" s="2">
         <v>0.53692484417121944</v>
@@ -27235,7 +27235,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K21" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L21" s="2">
         <v>0.53692484417121944</v>
@@ -27300,7 +27300,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K22" s="2">
-        <v>4.1849314063524962E-2</v>
+        <v>4.1849314063524892E-2</v>
       </c>
       <c r="L22" s="2">
         <v>0.53692484417121944</v>
@@ -27365,7 +27365,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K23" s="2">
-        <v>0.50884411637355365</v>
+        <v>0.50884411637355353</v>
       </c>
       <c r="L23" s="2">
         <v>0.53692484417121944</v>
@@ -27495,7 +27495,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K25" s="2">
-        <v>-0.29348857880586532</v>
+        <v>-0.29348857880586549</v>
       </c>
       <c r="L25" s="2">
         <v>0.53692484417121944</v>
@@ -27560,7 +27560,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K26" s="2">
-        <v>4.1849314063524962E-2</v>
+        <v>4.1849314063524892E-2</v>
       </c>
       <c r="L26" s="2">
         <v>0.53692484417121944</v>
@@ -27690,7 +27690,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K28" s="2">
-        <v>0.59171052408030833</v>
+        <v>0.59171052408030811</v>
       </c>
       <c r="L28" s="2">
         <v>0.53692484417121944</v>
@@ -27755,7 +27755,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K29" s="2">
-        <v>0.71329955221078001</v>
+        <v>0.7132995522107799</v>
       </c>
       <c r="L29" s="2">
         <v>0.53692484417121944</v>
@@ -27820,7 +27820,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K30" s="2">
-        <v>1.123759328702181</v>
+        <v>1.1237593287021821</v>
       </c>
       <c r="L30" s="2">
         <v>-1.8624580532189181</v>
@@ -27950,7 +27950,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K32" s="2">
-        <v>0.45463244778034939</v>
+        <v>0.4546324477803495</v>
       </c>
       <c r="L32" s="2">
         <v>0.53692484417121944</v>
@@ -28015,7 +28015,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K33" s="2">
-        <v>0.88058127244123785</v>
+        <v>0.88058127244123796</v>
       </c>
       <c r="L33" s="2">
         <v>-1.8624580532189181</v>
@@ -28080,7 +28080,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K34" s="2">
-        <v>0.5971316909396287</v>
+        <v>0.59713169093962859</v>
       </c>
       <c r="L34" s="2">
         <v>0.53692484417121944</v>
@@ -28145,7 +28145,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K35" s="2">
-        <v>0.19673979575839351</v>
+        <v>0.1967397957583934</v>
       </c>
       <c r="L35" s="2">
         <v>0.53692484417121944</v>
@@ -28275,7 +28275,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K37" s="2">
-        <v>4.1849314063524962E-2</v>
+        <v>4.1849314063524892E-2</v>
       </c>
       <c r="L37" s="2">
         <v>0.53692484417121944</v>
@@ -28405,7 +28405,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K39" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L39" s="2">
         <v>0.53692484417121944</v>
@@ -28535,7 +28535,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K41" s="2">
-        <v>0.17892739036348379</v>
+        <v>0.17892739036348351</v>
       </c>
       <c r="L41" s="2">
         <v>-1.8624580532189181</v>
@@ -28600,7 +28600,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K42" s="2">
-        <v>-0.12620685857540759</v>
+        <v>-0.12620685857540739</v>
       </c>
       <c r="L42" s="2">
         <v>0.53692484417121944</v>
@@ -28665,7 +28665,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K43" s="2">
-        <v>0.65366671675825549</v>
+        <v>0.65366671675825561</v>
       </c>
       <c r="L43" s="2">
         <v>0.53692484417121944</v>
@@ -28730,7 +28730,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K44" s="2">
-        <v>-0.37093381965329952</v>
+        <v>-0.37093381965329969</v>
       </c>
       <c r="L44" s="2">
         <v>0.53692484417121944</v>
@@ -28860,7 +28860,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K46" s="2">
-        <v>-0.1773207175347139</v>
+        <v>-0.1773207175347141</v>
       </c>
       <c r="L46" s="2">
         <v>0.53692484417121944</v>
@@ -28925,7 +28925,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K47" s="2">
-        <v>0.39577406473629961</v>
+        <v>0.3957740647362995</v>
       </c>
       <c r="L47" s="2">
         <v>0.53692484417121944</v>
@@ -28990,7 +28990,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K48" s="2">
-        <v>-0.70704616493116457</v>
+        <v>-0.70704616493116434</v>
       </c>
       <c r="L48" s="2">
         <v>0.53692484417121944</v>
@@ -29120,7 +29120,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K50" s="2">
-        <v>-0.3748060816956717</v>
+        <v>-0.37480608169567148</v>
       </c>
       <c r="L50" s="2">
         <v>0.53692484417121944</v>
@@ -29185,7 +29185,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K51" s="2">
-        <v>-0.37093381965329952</v>
+        <v>-0.37093381965329969</v>
       </c>
       <c r="L51" s="2">
         <v>0.53692484417121944</v>
@@ -29250,7 +29250,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K52" s="2">
-        <v>0.36402151598885119</v>
+        <v>0.36402151598885141</v>
       </c>
       <c r="L52" s="2">
         <v>0.53692484417121944</v>
@@ -29315,7 +29315,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K53" s="2">
-        <v>0.51658864045829722</v>
+        <v>0.51658864045829689</v>
       </c>
       <c r="L53" s="2">
         <v>0.53692484417121944</v>
@@ -29445,7 +29445,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K55" s="2">
-        <v>-0.61643523313966619</v>
+        <v>-0.61643523313966631</v>
       </c>
       <c r="L55" s="2">
         <v>0.53692484417121944</v>
@@ -29575,7 +29575,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K57" s="2">
-        <v>-0.38952067745668389</v>
+        <v>-0.38952067745668401</v>
       </c>
       <c r="L57" s="2">
         <v>0.53692484417121944</v>
@@ -29705,7 +29705,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K59" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L59" s="2">
         <v>-1.8624580532189181</v>
@@ -29770,7 +29770,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K60" s="2">
-        <v>0.42907551830069629</v>
+        <v>0.42907551830069618</v>
       </c>
       <c r="L60" s="2">
         <v>-1.8624580532189181</v>
@@ -29965,7 +29965,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K63" s="2">
-        <v>-0.13859809711099669</v>
+        <v>-0.13859809711099691</v>
       </c>
       <c r="L63" s="2">
         <v>0.53692484417121944</v>
@@ -30160,7 +30160,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K66" s="2">
-        <v>0.63430540654639689</v>
+        <v>0.634305406546397</v>
       </c>
       <c r="L66" s="2">
         <v>0.53692484417121944</v>
@@ -30225,7 +30225,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K67" s="2">
-        <v>0.1711828662787403</v>
+        <v>0.1711828662787401</v>
       </c>
       <c r="L67" s="2">
         <v>0.53692484417121944</v>
@@ -30355,7 +30355,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K69" s="2">
-        <v>0.84185865201752064</v>
+        <v>0.84185865201752086</v>
       </c>
       <c r="L69" s="2">
         <v>0.53692484417121944</v>
@@ -30420,7 +30420,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K70" s="2">
-        <v>-1.623461657205073E-2</v>
+        <v>-1.6234616572050799E-2</v>
       </c>
       <c r="L70" s="2">
         <v>0.53692484417121944</v>
@@ -30485,7 +30485,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K71" s="2">
-        <v>-0.50801189595325824</v>
+        <v>-0.50801189595325835</v>
       </c>
       <c r="L71" s="2">
         <v>0.53692484417121944</v>
@@ -30615,7 +30615,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K73" s="2">
-        <v>0.48561054411932297</v>
+        <v>0.48561054411932331</v>
       </c>
       <c r="L73" s="2">
         <v>0.53692484417121944</v>
@@ -30680,7 +30680,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K74" s="2">
-        <v>0.1138733880516388</v>
+        <v>0.1138733880516387</v>
       </c>
       <c r="L74" s="2">
         <v>0.53692484417121944</v>
@@ -30745,7 +30745,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K75" s="2">
-        <v>0.3462091105939416</v>
+        <v>0.34620911059394149</v>
       </c>
       <c r="L75" s="2">
         <v>0.53692484417121944</v>
@@ -30810,7 +30810,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K76" s="2">
-        <v>0.7163973618446775</v>
+        <v>0.71639736184467739</v>
       </c>
       <c r="L76" s="2">
         <v>0.53692484417121944</v>
@@ -30940,7 +30940,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K78" s="2">
-        <v>-0.23153238612791791</v>
+        <v>-0.23153238612791799</v>
       </c>
       <c r="L78" s="2">
         <v>0.53692484417121944</v>
@@ -31005,7 +31005,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K79" s="2">
-        <v>-0.72485857032607415</v>
+        <v>-0.72485857032607426</v>
       </c>
       <c r="L79" s="2">
         <v>0.53692484417121944</v>
@@ -31200,7 +31200,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K82" s="2">
-        <v>-0.33221119922958242</v>
+        <v>-0.33221119922958259</v>
       </c>
       <c r="L82" s="2">
         <v>0.53692484417121944</v>
@@ -31265,7 +31265,7 @@
         <v>1.701379756343312</v>
       </c>
       <c r="K83" s="2">
-        <v>-9.987547668727953E-2</v>
+        <v>-9.9875476687279807E-2</v>
       </c>
       <c r="L83" s="2">
         <v>-1.8624580532189181</v>
@@ -31330,7 +31330,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K84" s="2">
-        <v>5.5015005007588921E-2</v>
+        <v>5.5015005007588713E-2</v>
       </c>
       <c r="L84" s="2">
         <v>0.53692484417121944</v>
@@ -31395,7 +31395,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K85" s="2">
-        <v>-0.31981996069399321</v>
+        <v>-0.3198199606939931</v>
       </c>
       <c r="L85" s="2">
         <v>0.53692484417121944</v>
@@ -31460,7 +31460,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K86" s="2">
-        <v>-0.53898999229223199</v>
+        <v>-0.5389899922922321</v>
       </c>
       <c r="L86" s="2">
         <v>0.53692484417121944</v>
@@ -31525,7 +31525,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K87" s="2">
-        <v>0.14485148439061241</v>
+        <v>0.14485148439061249</v>
       </c>
       <c r="L87" s="2">
         <v>0.53692484417121944</v>
@@ -31785,7 +31785,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K91" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L91" s="2">
         <v>0.53692484417121944</v>
@@ -31850,7 +31850,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K92" s="2">
-        <v>9.9933244699100657E-2</v>
+        <v>9.9933244699100587E-2</v>
       </c>
       <c r="L92" s="2">
         <v>-1.8624580532189181</v>
@@ -31915,7 +31915,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K93" s="2">
-        <v>-0.31284988901772381</v>
+        <v>-0.31284988901772398</v>
       </c>
       <c r="L93" s="2">
         <v>0.53692484417121944</v>
@@ -32045,7 +32045,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K95" s="2">
-        <v>-0.54441115915155236</v>
+        <v>-0.54441115915155247</v>
       </c>
       <c r="L95" s="2">
         <v>0.53692484417121944</v>
@@ -32175,7 +32175,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K97" s="2">
-        <v>0.2617937980702385</v>
+        <v>0.26179379807023823</v>
       </c>
       <c r="L97" s="2">
         <v>-1.8624580532189181</v>
@@ -32240,7 +32240,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K98" s="2">
-        <v>-8.6709785743215709E-2</v>
+        <v>-8.6709785743215986E-2</v>
       </c>
       <c r="L98" s="2">
         <v>0.53692484417121944</v>
@@ -32370,7 +32370,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K100" s="2">
-        <v>0.72569079074636933</v>
+        <v>0.72569079074636944</v>
       </c>
       <c r="L100" s="2">
         <v>0.53692484417121944</v>
@@ -32435,7 +32435,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K101" s="2">
-        <v>0.15801717533467641</v>
+        <v>0.1580171753346763</v>
       </c>
       <c r="L101" s="2">
         <v>0.53692484417121944</v>
@@ -32500,7 +32500,7 @@
         <v>0.57673890045536014</v>
       </c>
       <c r="K102" s="2">
-        <v>0.53285214103625844</v>
+        <v>0.53285214103625811</v>
       </c>
       <c r="L102" s="2">
         <v>0.53692484417121944</v>
@@ -32565,7 +32565,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K103" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L103" s="2">
         <v>0.53692484417121944</v>
@@ -32630,7 +32630,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K104" s="2">
-        <v>0.15801717533467641</v>
+        <v>0.1580171753346763</v>
       </c>
       <c r="L104" s="2">
         <v>0.53692484417121944</v>
@@ -32695,7 +32695,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K105" s="2">
-        <v>0.46779813872441339</v>
+        <v>0.46779813872441328</v>
       </c>
       <c r="L105" s="2">
         <v>0.53692484417121944</v>
@@ -32825,7 +32825,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K107" s="2">
-        <v>0.61262073910911585</v>
+        <v>0.61262073910911541</v>
       </c>
       <c r="L107" s="2">
         <v>-1.8624580532189181</v>
@@ -32890,7 +32890,7 @@
         <v>-0.54790195543259212</v>
       </c>
       <c r="K108" s="2">
-        <v>-0.30665426974992921</v>
+        <v>-0.30665426974992932</v>
       </c>
       <c r="L108" s="2">
         <v>0.53692484417121944</v>

</xml_diff>

<commit_message>
code done for POC, tesis readt 4 pendrive
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80D5FB5-BE5D-4606-9876-FDB7648AF2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18377A58-60A2-4086-88D9-B42B3D2998C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="0" windowWidth="12000" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
improved font on sns heatcorrelation map
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18377A58-60A2-4086-88D9-B42B3D2998C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA513D4F-E5CC-43AE-BD69-F99B4DC0D8B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
DT added label option
</commit_message>
<xml_diff>
--- a/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
+++ b/results/ML/DT_cEnroll_nPSU_nS1S2_vs_Desertor/DT_train.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\models\desertorstudent\results\ML\DT_cEnroll_nPSU_nS1S2_vs_Desertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA513D4F-E5CC-43AE-BD69-F99B4DC0D8B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A621BE8-B8A4-419B-83AB-97FF9333A784}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="0" windowWidth="16800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="train" sheetId="1" r:id="rId1"/>

</xml_diff>